<commit_message>
Sun Mar  9 17:45:37 CET 2025
</commit_message>
<xml_diff>
--- a/_GPO/Project Manager/Project Controller 5IB_n_X.xlsx
+++ b/_GPO/Project Manager/Project Controller 5IB_n_X.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/origgi/Desktop/StefanoOriggi/_GPO/Project Manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E995029-5F06-2D48-ACEA-3935FFFAB6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5696818D-10EB-5246-B1F5-1B9DA6578094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="100">
   <si>
     <t>Monitoraggio e Controllo Globale</t>
   </si>
@@ -299,12 +299,6 @@
     <t>Anticipo</t>
   </si>
   <si>
-    <t>OBS</t>
-  </si>
-  <si>
-    <t>WBS</t>
-  </si>
-  <si>
     <t>RAM</t>
   </si>
   <si>
@@ -342,6 +336,9 @@
   </si>
   <si>
     <t>GANNT DI PROGETTO</t>
+  </si>
+  <si>
+    <t>I WORKING PAPERS</t>
   </si>
 </sst>
 </file>
@@ -973,6 +970,153 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -981,153 +1125,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1553,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScale="118" zoomScaleNormal="100" zoomScalePageLayoutView="118" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A34" zoomScale="118" zoomScaleNormal="100" zoomScalePageLayoutView="118" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1573,15 +1570,15 @@
       <c r="A1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
       <c r="I1" s="27"/>
       <c r="J1" s="25" t="s">
         <v>1</v>
@@ -1591,84 +1588,84 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:12" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="78"/>
       <c r="G3" s="28">
         <f>WEEKNUM(I6)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="73"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="29">
         <f>G3+2</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="79" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="67" t="s">
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="68"/>
-      <c r="K5" s="69"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1687,17 +1684,17 @@
       <c r="H6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="50">
-        <v>45712</v>
-      </c>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
+      <c r="I6" s="68">
+        <v>45730</v>
+      </c>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="86"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
@@ -1716,74 +1713,74 @@
       <c r="H7" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="86"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="74"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="76"/>
-      <c r="I8" s="67" t="s">
+      <c r="H8" s="82"/>
+      <c r="I8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="76"/>
       <c r="L8" s="24"/>
     </row>
     <row r="9" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="86"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="75"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="75"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="77"/>
-      <c r="I9" s="50">
-        <v>45718</v>
-      </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="68">
+        <v>45738</v>
+      </c>
+      <c r="J9" s="69"/>
+      <c r="K9" s="70"/>
     </row>
     <row r="10" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="54">
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="88">
         <f>I9-2</f>
-        <v>45716</v>
-      </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+        <v>45736</v>
+      </c>
+      <c r="J10" s="89"/>
+      <c r="K10" s="90"/>
     </row>
     <row r="11" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1799,61 +1796,61 @@
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:12" s="19" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="60"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="93"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="82" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="57"/>
-      <c r="J13" s="53" t="s">
+      <c r="I13" s="48"/>
+      <c r="J13" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="53"/>
+      <c r="K13" s="47"/>
     </row>
     <row r="14" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="70"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="82"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
     </row>
     <row r="15" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
@@ -1862,12 +1859,12 @@
       <c r="B15" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="96"/>
       <c r="G15" s="22" t="s">
         <v>21</v>
       </c>
@@ -1877,10 +1874,10 @@
       <c r="I15" s="21">
         <v>11</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="46">
         <v>1</v>
       </c>
-      <c r="K15" s="49"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1889,12 +1886,12 @@
       <c r="B16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
+      <c r="C16" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="22" t="s">
         <v>21</v>
       </c>
@@ -1904,10 +1901,10 @@
       <c r="I16" s="21">
         <v>13</v>
       </c>
-      <c r="J16" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="K16" s="49"/>
+      <c r="J16" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="K16" s="46"/>
     </row>
     <row r="17" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1916,12 +1913,12 @@
       <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
+      <c r="C17" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="22" t="s">
         <v>21</v>
       </c>
@@ -1931,10 +1928,10 @@
       <c r="I17" s="21">
         <v>16</v>
       </c>
-      <c r="J17" s="49">
-        <v>0.3</v>
-      </c>
-      <c r="K17" s="49"/>
+      <c r="J17" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="46"/>
     </row>
     <row r="18" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -1943,25 +1940,25 @@
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
+      <c r="C18" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I18" s="21">
-        <v>10</v>
-      </c>
-      <c r="J18" s="49">
-        <v>0.4</v>
-      </c>
-      <c r="K18" s="49"/>
+        <v>12</v>
+      </c>
+      <c r="J18" s="46">
+        <v>1</v>
+      </c>
+      <c r="K18" s="46"/>
     </row>
     <row r="19" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -1970,25 +1967,25 @@
       <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
+      <c r="C19" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="21">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I19" s="21">
-        <v>10</v>
-      </c>
-      <c r="J19" s="49">
+        <v>14</v>
+      </c>
+      <c r="J19" s="46">
         <v>1</v>
       </c>
-      <c r="K19" s="49"/>
+      <c r="K19" s="46"/>
     </row>
     <row r="20" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -1997,25 +1994,25 @@
       <c r="B20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+      <c r="C20" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I20" s="21">
-        <v>10</v>
-      </c>
-      <c r="J20" s="49">
+        <v>12</v>
+      </c>
+      <c r="J20" s="46">
         <v>1</v>
       </c>
-      <c r="K20" s="49"/>
+      <c r="K20" s="46"/>
     </row>
     <row r="21" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -2024,25 +2021,25 @@
       <c r="B21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
+      <c r="C21" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I21" s="21">
-        <v>11</v>
-      </c>
-      <c r="J21" s="49">
-        <v>0.8</v>
-      </c>
-      <c r="K21" s="49"/>
+        <v>12</v>
+      </c>
+      <c r="J21" s="46">
+        <v>1</v>
+      </c>
+      <c r="K21" s="46"/>
     </row>
     <row r="22" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -2051,12 +2048,12 @@
       <c r="B22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
+      <c r="C22" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="22" t="s">
         <v>85</v>
       </c>
@@ -2066,82 +2063,82 @@
       <c r="I22" s="21">
         <v>14</v>
       </c>
-      <c r="J22" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="K22" s="49"/>
+      <c r="J22" s="46">
+        <v>0.8</v>
+      </c>
+      <c r="K22" s="46"/>
     </row>
     <row r="23" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="22"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
     </row>
     <row r="24" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="91" t="s">
+      <c r="A24" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="93"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="56"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="82" t="s">
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="57" t="s">
+      <c r="H25" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="57"/>
-      <c r="J25" s="53" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="53"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="70"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="82"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
@@ -2150,25 +2147,25 @@
       <c r="B27" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
+      <c r="C27" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I27" s="21">
-        <v>11</v>
-      </c>
-      <c r="J27" s="49">
+        <v>12</v>
+      </c>
+      <c r="J27" s="46">
         <v>1</v>
       </c>
-      <c r="K27" s="49"/>
+      <c r="K27" s="46"/>
     </row>
     <row r="28" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -2177,12 +2174,12 @@
       <c r="B28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
+      <c r="C28" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="22" t="s">
         <v>21</v>
       </c>
@@ -2192,10 +2189,10 @@
       <c r="I28" s="21">
         <v>14</v>
       </c>
-      <c r="J28" s="49">
-        <v>0.3</v>
-      </c>
-      <c r="K28" s="49"/>
+      <c r="J28" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="46"/>
     </row>
     <row r="29" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -2204,12 +2201,12 @@
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
+      <c r="C29" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="22" t="s">
         <v>21</v>
       </c>
@@ -2219,10 +2216,10 @@
       <c r="I29" s="21">
         <v>13</v>
       </c>
-      <c r="J29" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="K29" s="49"/>
+      <c r="J29" s="46">
+        <v>0.6</v>
+      </c>
+      <c r="K29" s="46"/>
     </row>
     <row r="30" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -2231,12 +2228,12 @@
       <c r="B30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
+      <c r="C30" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="22" t="s">
         <v>21</v>
       </c>
@@ -2246,10 +2243,10 @@
       <c r="I30" s="21">
         <v>11</v>
       </c>
-      <c r="J30" s="49">
-        <v>0.9</v>
-      </c>
-      <c r="K30" s="49"/>
+      <c r="J30" s="46">
+        <v>1</v>
+      </c>
+      <c r="K30" s="46"/>
     </row>
     <row r="31" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -2258,12 +2255,12 @@
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
+      <c r="C31" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="22" t="s">
         <v>21</v>
       </c>
@@ -2273,10 +2270,10 @@
       <c r="I31" s="21">
         <v>13</v>
       </c>
-      <c r="J31" s="49">
-        <v>0.6</v>
-      </c>
-      <c r="K31" s="49"/>
+      <c r="J31" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="K31" s="46"/>
     </row>
     <row r="32" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -2285,12 +2282,12 @@
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
+      <c r="C32" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="22" t="s">
         <v>21</v>
       </c>
@@ -2300,10 +2297,10 @@
       <c r="I32" s="21">
         <v>12</v>
       </c>
-      <c r="J32" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="K32" s="49"/>
+      <c r="J32" s="46">
+        <v>1</v>
+      </c>
+      <c r="K32" s="46"/>
     </row>
     <row r="33" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -2312,25 +2309,25 @@
       <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
+      <c r="C33" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="21">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I33" s="21">
-        <v>10</v>
-      </c>
-      <c r="J33" s="49">
-        <v>1</v>
-      </c>
-      <c r="K33" s="49"/>
+        <v>14</v>
+      </c>
+      <c r="J33" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="K33" s="46"/>
     </row>
     <row r="34" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -2339,97 +2336,97 @@
       <c r="B34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
+      <c r="C34" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="21">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I34" s="21">
-        <v>11</v>
-      </c>
-      <c r="J34" s="49">
-        <v>1</v>
-      </c>
-      <c r="K34" s="49"/>
+        <v>15</v>
+      </c>
+      <c r="J34" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="K34" s="46"/>
     </row>
     <row r="35" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="22"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
     </row>
     <row r="37" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="96"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="82" t="s">
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="57" t="s">
+      <c r="H38" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="57"/>
-      <c r="J38" s="53" t="s">
+      <c r="I38" s="48"/>
+      <c r="J38" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="K38" s="53"/>
+      <c r="K38" s="47"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="70"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="82"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
     </row>
     <row r="40" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
@@ -2438,12 +2435,12 @@
       <c r="B40" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
+      <c r="C40" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
       <c r="G40" s="22" t="s">
         <v>21</v>
       </c>
@@ -2453,10 +2450,10 @@
       <c r="I40" s="21">
         <v>11</v>
       </c>
-      <c r="J40" s="49">
+      <c r="J40" s="46">
         <v>1</v>
       </c>
-      <c r="K40" s="49"/>
+      <c r="K40" s="46"/>
     </row>
     <row r="41" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -2465,25 +2462,25 @@
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
+      <c r="C41" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H41" s="21">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I41" s="21">
-        <v>11</v>
-      </c>
-      <c r="J41" s="49">
-        <v>1</v>
-      </c>
-      <c r="K41" s="49"/>
+        <v>13</v>
+      </c>
+      <c r="J41" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="K41" s="46"/>
     </row>
     <row r="42" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -2492,25 +2489,25 @@
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
+      <c r="C42" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
       <c r="G42" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="21">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I42" s="21">
-        <v>11</v>
-      </c>
-      <c r="J42" s="49">
-        <v>1</v>
-      </c>
-      <c r="K42" s="49"/>
+        <v>13</v>
+      </c>
+      <c r="J42" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="46"/>
     </row>
     <row r="43" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -2519,12 +2516,12 @@
       <c r="B43" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
+      <c r="C43" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
       <c r="G43" s="22" t="s">
         <v>21</v>
       </c>
@@ -2534,10 +2531,10 @@
       <c r="I43" s="21">
         <v>13</v>
       </c>
-      <c r="J43" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="K43" s="49"/>
+      <c r="J43" s="46">
+        <v>0.8</v>
+      </c>
+      <c r="K43" s="46"/>
     </row>
     <row r="44" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -2546,12 +2543,12 @@
       <c r="B44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
+      <c r="C44" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
       <c r="G44" s="22" t="s">
         <v>21</v>
       </c>
@@ -2561,10 +2558,10 @@
       <c r="I44" s="21">
         <v>13</v>
       </c>
-      <c r="J44" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="K44" s="49"/>
+      <c r="J44" s="46">
+        <v>0.8</v>
+      </c>
+      <c r="K44" s="46"/>
     </row>
     <row r="45" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -2573,12 +2570,12 @@
       <c r="B45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
+      <c r="C45" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
       <c r="G45" s="22" t="s">
         <v>21</v>
       </c>
@@ -2588,10 +2585,10 @@
       <c r="I45" s="21">
         <v>12</v>
       </c>
-      <c r="J45" s="49">
-        <v>0.8</v>
-      </c>
-      <c r="K45" s="49"/>
+      <c r="J45" s="46">
+        <v>1</v>
+      </c>
+      <c r="K45" s="46"/>
     </row>
     <row r="46" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -2600,12 +2597,12 @@
       <c r="B46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
+      <c r="C46" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
       <c r="G46" s="22" t="s">
         <v>21</v>
       </c>
@@ -2615,99 +2612,67 @@
       <c r="I46" s="21">
         <v>12</v>
       </c>
-      <c r="J46" s="49">
-        <v>0.8</v>
-      </c>
-      <c r="K46" s="49"/>
+      <c r="J46" s="46">
+        <v>1</v>
+      </c>
+      <c r="K46" s="46"/>
     </row>
     <row r="47" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
       <c r="G47" s="22"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
     </row>
     <row r="48" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
       <c r="G48" s="22"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J38:K39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K26"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I6:K7"/>
     <mergeCell ref="I8:K8"/>
@@ -2724,30 +2689,62 @@
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="J13:K14"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
   </mergeCells>
   <phoneticPr fontId="28" type="noConversion"/>
   <conditionalFormatting sqref="C8 E8 G8 G15:G23">
@@ -4155,12 +4152,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4359,20 +4358,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{037C351A-E6D8-4630-8C6B-3FB347BAF71A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98743F9B-98B2-46F4-A3B1-3476BE7E5D56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
+    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4397,12 +4397,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98743F9B-98B2-46F4-A3B1-3476BE7E5D56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{037C351A-E6D8-4630-8C6B-3FB347BAF71A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
-    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sat Apr 12 13:38:01 CEST 2025
</commit_message>
<xml_diff>
--- a/_GPO/Project Manager/Project Controller 5IB_n_X.xlsx
+++ b/_GPO/Project Manager/Project Controller 5IB_n_X.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/origgi/Desktop/StefanoOriggi/_GPO/Project Manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5696818D-10EB-5246-B1F5-1B9DA6578094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590E743-B651-3347-9E31-6881CFEEA914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,33 +296,12 @@
     <t>5IB</t>
   </si>
   <si>
-    <t>Anticipo</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>GANTT DI PROGETTO</t>
-  </si>
-  <si>
-    <t>PIANO DEI RILASCI</t>
-  </si>
-  <si>
-    <t>BUDGET DI PROGETTO</t>
-  </si>
-  <si>
-    <t>PIANO DELLE RISORSE</t>
-  </si>
-  <si>
     <t xml:space="preserve">ORGANIZZAZIONE TEAM </t>
   </si>
   <si>
     <t>ORGANIZZAZIONE TEAM</t>
   </si>
   <si>
-    <t>PIANO DELLA QUALITÀ</t>
-  </si>
-  <si>
     <t>PIANI DI PROJECT MANAGEMENT</t>
   </si>
   <si>
@@ -335,10 +314,31 @@
     <t>PIANO DEGLI APPROVIGIONAMENTI</t>
   </si>
   <si>
-    <t>GANNT DI PROGETTO</t>
-  </si>
-  <si>
     <t>I WORKING PAPERS</t>
+  </si>
+  <si>
+    <t>I REPORT DEI TEST DI ACCETTAZIONE</t>
+  </si>
+  <si>
+    <t>IL REPORT DI STATO AVANZAMENTO LAVORI</t>
+  </si>
+  <si>
+    <t>WORKING PAPERS</t>
+  </si>
+  <si>
+    <t>FINITO</t>
+  </si>
+  <si>
+    <t>REPORT FINALE</t>
+  </si>
+  <si>
+    <t>PROCEDURA DI GESTIONE DELLE MODIFICHE</t>
+  </si>
+  <si>
+    <t>PIANO DELLE COMUNICAZIONE</t>
+  </si>
+  <si>
+    <t>REPORT DI STATO AVANZAMENTO</t>
   </si>
 </sst>
 </file>
@@ -970,40 +970,121 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1027,104 +1108,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A34" zoomScale="118" zoomScaleNormal="100" zoomScalePageLayoutView="118" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A21" zoomScale="118" zoomScaleNormal="100" zoomScalePageLayoutView="118" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1570,15 +1570,15 @@
       <c r="A1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="63"/>
       <c r="I1" s="27"/>
       <c r="J1" s="25" t="s">
         <v>1</v>
@@ -1588,84 +1588,84 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
     </row>
     <row r="3" spans="1:12" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="78"/>
+      <c r="F3" s="72"/>
       <c r="G3" s="28">
         <f>WEEKNUM(I6)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="79"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="29">
         <f>G3+2</f>
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="85" t="s">
+      <c r="B5" s="85"/>
+      <c r="C5" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="74" t="s">
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="76"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1684,17 +1684,17 @@
       <c r="H6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="68">
-        <v>45730</v>
-      </c>
-      <c r="J6" s="69"/>
-      <c r="K6" s="70"/>
+      <c r="I6" s="50">
+        <v>45761</v>
+      </c>
+      <c r="J6" s="51"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
@@ -1713,74 +1713,74 @@
       <c r="H7" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="80"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="74"/>
       <c r="G8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="82"/>
-      <c r="I8" s="74" t="s">
+      <c r="H8" s="76"/>
+      <c r="I8" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="75"/>
-      <c r="K8" s="76"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="24"/>
     </row>
     <row r="9" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="81"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="75"/>
       <c r="G9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="83"/>
-      <c r="I9" s="68">
-        <v>45738</v>
-      </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="50">
+        <v>45768</v>
+      </c>
+      <c r="J9" s="51"/>
+      <c r="K9" s="52"/>
     </row>
     <row r="10" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="88">
+      <c r="B10" s="87"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="54">
         <f>I9-2</f>
-        <v>45736</v>
-      </c>
-      <c r="J10" s="89"/>
-      <c r="K10" s="90"/>
+        <v>45766</v>
+      </c>
+      <c r="J10" s="55"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1796,61 +1796,61 @@
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:12" s="19" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="93"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="50" t="s">
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="48"/>
-      <c r="J13" s="47" t="s">
+      <c r="I13" s="57"/>
+      <c r="J13" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="47"/>
+      <c r="K13" s="53"/>
     </row>
     <row r="14" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="50"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
@@ -1859,25 +1859,25 @@
       <c r="B15" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="94" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="96"/>
+      <c r="C15" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="21">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I15" s="21">
-        <v>11</v>
-      </c>
-      <c r="J15" s="46">
+        <v>16</v>
+      </c>
+      <c r="J15" s="49">
         <v>1</v>
       </c>
-      <c r="K15" s="46"/>
+      <c r="K15" s="49"/>
     </row>
     <row r="16" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1886,25 +1886,25 @@
       <c r="B16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="94" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="96"/>
+      <c r="C16" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
       <c r="G16" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="21">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I16" s="21">
-        <v>13</v>
-      </c>
-      <c r="J16" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="K16" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="J16" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="K16" s="49"/>
     </row>
     <row r="17" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1913,12 +1913,12 @@
       <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="94" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="96"/>
+      <c r="C17" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="22" t="s">
         <v>21</v>
       </c>
@@ -1928,10 +1928,10 @@
       <c r="I17" s="21">
         <v>16</v>
       </c>
-      <c r="J17" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="K17" s="46"/>
+      <c r="J17" s="49">
+        <v>0.9</v>
+      </c>
+      <c r="K17" s="49"/>
     </row>
     <row r="18" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -1940,25 +1940,25 @@
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="94" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="96"/>
+      <c r="C18" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="21">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I18" s="21">
-        <v>12</v>
-      </c>
-      <c r="J18" s="46">
+        <v>15</v>
+      </c>
+      <c r="J18" s="49">
         <v>1</v>
       </c>
-      <c r="K18" s="46"/>
+      <c r="K18" s="49"/>
     </row>
     <row r="19" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -1967,25 +1967,25 @@
       <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="94" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="96"/>
+      <c r="C19" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="21">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I19" s="21">
-        <v>14</v>
-      </c>
-      <c r="J19" s="46">
+        <v>16</v>
+      </c>
+      <c r="J19" s="49">
         <v>1</v>
       </c>
-      <c r="K19" s="46"/>
+      <c r="K19" s="49"/>
     </row>
     <row r="20" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -1994,25 +1994,25 @@
       <c r="B20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
+      <c r="C20" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
       <c r="G20" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="21">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I20" s="21">
-        <v>12</v>
-      </c>
-      <c r="J20" s="46">
-        <v>1</v>
-      </c>
-      <c r="K20" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="J20" s="49">
+        <v>0.8</v>
+      </c>
+      <c r="K20" s="49"/>
     </row>
     <row r="21" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -2021,25 +2021,25 @@
       <c r="B21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
+      <c r="C21" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="21">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I21" s="21">
-        <v>12</v>
-      </c>
-      <c r="J21" s="46">
-        <v>1</v>
-      </c>
-      <c r="K21" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="J21" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="K21" s="49"/>
     </row>
     <row r="22" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -2048,97 +2048,97 @@
       <c r="B22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
+      <c r="C22" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
       <c r="G22" s="22" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="H22" s="21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I22" s="21">
-        <v>14</v>
-      </c>
-      <c r="J22" s="46">
-        <v>0.8</v>
-      </c>
-      <c r="K22" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="J22" s="49">
+        <v>1</v>
+      </c>
+      <c r="K22" s="49"/>
     </row>
     <row r="23" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
       <c r="G23" s="22"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="93"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="50" t="s">
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="48"/>
-      <c r="J25" s="47" t="s">
+      <c r="I25" s="57"/>
+      <c r="J25" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="47"/>
+      <c r="K25" s="53"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="50"/>
+      <c r="A26" s="70"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="82"/>
       <c r="H26" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
     </row>
     <row r="27" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
@@ -2147,25 +2147,25 @@
       <c r="B27" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
+      <c r="C27" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
       <c r="G27" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="21">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I27" s="21">
-        <v>12</v>
-      </c>
-      <c r="J27" s="46">
+        <v>16</v>
+      </c>
+      <c r="J27" s="49">
         <v>1</v>
       </c>
-      <c r="K27" s="46"/>
+      <c r="K27" s="49"/>
     </row>
     <row r="28" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -2174,25 +2174,25 @@
       <c r="B28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
+      <c r="C28" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
       <c r="G28" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H28" s="21">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I28" s="21">
-        <v>14</v>
-      </c>
-      <c r="J28" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="K28" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J28" s="49">
+        <v>1</v>
+      </c>
+      <c r="K28" s="49"/>
     </row>
     <row r="29" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -2201,25 +2201,25 @@
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
+      <c r="C29" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
       <c r="G29" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H29" s="21">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I29" s="21">
-        <v>13</v>
-      </c>
-      <c r="J29" s="46">
-        <v>0.6</v>
-      </c>
-      <c r="K29" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="J29" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="K29" s="49"/>
     </row>
     <row r="30" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -2228,25 +2228,25 @@
       <c r="B30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
+      <c r="C30" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
       <c r="G30" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H30" s="21">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I30" s="21">
-        <v>11</v>
-      </c>
-      <c r="J30" s="46">
-        <v>1</v>
-      </c>
-      <c r="K30" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J30" s="49">
+        <v>0.8</v>
+      </c>
+      <c r="K30" s="49"/>
     </row>
     <row r="31" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -2255,25 +2255,25 @@
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
+      <c r="C31" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="21">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I31" s="21">
-        <v>13</v>
-      </c>
-      <c r="J31" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="K31" s="46"/>
+        <v>17</v>
+      </c>
+      <c r="J31" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="K31" s="49"/>
     </row>
     <row r="32" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -2282,25 +2282,25 @@
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
+      <c r="C32" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H32" s="21">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I32" s="21">
-        <v>12</v>
-      </c>
-      <c r="J32" s="46">
-        <v>1</v>
-      </c>
-      <c r="K32" s="46"/>
+        <v>17</v>
+      </c>
+      <c r="J32" s="49">
+        <v>0.8</v>
+      </c>
+      <c r="K32" s="49"/>
     </row>
     <row r="33" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -2309,25 +2309,25 @@
       <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
+      <c r="C33" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
       <c r="G33" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="21">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I33" s="21">
-        <v>14</v>
-      </c>
-      <c r="J33" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="K33" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J33" s="49">
+        <v>1</v>
+      </c>
+      <c r="K33" s="49"/>
     </row>
     <row r="34" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -2336,97 +2336,97 @@
       <c r="B34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
+      <c r="C34" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
       <c r="G34" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I34" s="21">
-        <v>15</v>
-      </c>
-      <c r="J34" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="K34" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J34" s="49">
+        <v>1</v>
+      </c>
+      <c r="K34" s="49"/>
     </row>
     <row r="35" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
       <c r="G35" s="22"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
     </row>
     <row r="37" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="53"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="95"/>
+      <c r="I37" s="95"/>
+      <c r="J37" s="95"/>
+      <c r="K37" s="96"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="50" t="s">
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="48" t="s">
+      <c r="H38" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="48"/>
-      <c r="J38" s="47" t="s">
+      <c r="I38" s="57"/>
+      <c r="J38" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K38" s="47"/>
+      <c r="K38" s="53"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="50"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="82"/>
       <c r="H39" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
     </row>
     <row r="40" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
@@ -2435,25 +2435,25 @@
       <c r="B40" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
+      <c r="C40" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
       <c r="G40" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H40" s="21">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I40" s="21">
-        <v>11</v>
-      </c>
-      <c r="J40" s="46">
+        <v>16</v>
+      </c>
+      <c r="J40" s="49">
         <v>1</v>
       </c>
-      <c r="K40" s="46"/>
+      <c r="K40" s="49"/>
     </row>
     <row r="41" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -2462,25 +2462,25 @@
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="C41" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
       <c r="G41" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H41" s="21">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I41" s="21">
-        <v>13</v>
-      </c>
-      <c r="J41" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="K41" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J41" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="K41" s="49"/>
     </row>
     <row r="42" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -2489,25 +2489,25 @@
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
+      <c r="C42" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
       <c r="G42" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="21">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I42" s="21">
-        <v>13</v>
-      </c>
-      <c r="J42" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="K42" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="J42" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="K42" s="49"/>
     </row>
     <row r="43" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -2516,25 +2516,25 @@
       <c r="B43" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
       <c r="G43" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H43" s="21">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I43" s="21">
-        <v>13</v>
-      </c>
-      <c r="J43" s="46">
-        <v>0.8</v>
-      </c>
-      <c r="K43" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="J43" s="49">
+        <v>0.9</v>
+      </c>
+      <c r="K43" s="49"/>
     </row>
     <row r="44" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -2543,25 +2543,25 @@
       <c r="B44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
       <c r="G44" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="21">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I44" s="21">
-        <v>13</v>
-      </c>
-      <c r="J44" s="46">
-        <v>0.8</v>
-      </c>
-      <c r="K44" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="J44" s="49">
+        <v>0.9</v>
+      </c>
+      <c r="K44" s="49"/>
     </row>
     <row r="45" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -2570,25 +2570,25 @@
       <c r="B45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
+      <c r="C45" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
       <c r="G45" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H45" s="21">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I45" s="21">
-        <v>12</v>
-      </c>
-      <c r="J45" s="46">
+        <v>15</v>
+      </c>
+      <c r="J45" s="49">
         <v>1</v>
       </c>
-      <c r="K45" s="46"/>
+      <c r="K45" s="49"/>
     </row>
     <row r="46" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -2597,66 +2597,130 @@
       <c r="B46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
+      <c r="C46" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
       <c r="G46" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H46" s="21">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I46" s="21">
-        <v>12</v>
-      </c>
-      <c r="J46" s="46">
+        <v>15</v>
+      </c>
+      <c r="J46" s="49">
         <v>1</v>
       </c>
-      <c r="K46" s="46"/>
+      <c r="K46" s="49"/>
     </row>
     <row r="47" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
       <c r="G47" s="22"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
     </row>
     <row r="48" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
       <c r="G48" s="22"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J38:K39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K26"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I6:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J18:K18"/>
@@ -2673,78 +2737,14 @@
     <mergeCell ref="C13:F14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I6:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <phoneticPr fontId="28" type="noConversion"/>
   <conditionalFormatting sqref="C8 E8 G8 G15:G23">
@@ -2853,7 +2853,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -4152,17 +4152,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C240D8F7A7575D4BACE6D8DC8CE2699D" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7bd0d3821f30cec562649af6727d5044">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb577c89-241a-4dd6-8c77-1faea3b86602" xmlns:ns3="b98c3651-2320-4920-a81d-baad65de77d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce9dba49ee2a04c2b3827884fb94a204" ns2:_="" ns3:_="">
     <xsd:import namespace="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
@@ -4357,6 +4346,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4367,17 +4367,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98743F9B-98B2-46F4-A3B1-3476BE7E5D56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
-    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E79697-FFED-4792-A241-6074DBB9495A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4396,6 +4385,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98743F9B-98B2-46F4-A3B1-3476BE7E5D56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
+    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{037C351A-E6D8-4630-8C6B-3FB347BAF71A}">
   <ds:schemaRefs>

</xml_diff>